<commit_message>
Add Dutch to YAML File
"convert_library_v1.py" has been used to ensure compatibility and avoid problems.
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/excel/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\ccb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D2251D-D3FE-46DF-8F8F-2B2A8B5A9135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C34A257-2480-4D4F-8E4A-413AD45D6DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2810" uniqueCount="2014">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="2011">
   <si>
     <t>assessable</t>
   </si>
@@ -6307,15 +6307,6 @@
 • Detectie en rapportage van atypisch gebruik van kritieke systemen van de organisatie. 
 • Het aanleggen van auditregistraties voor bepaalde informatie-/cyberbeveiligingsevents. 
 • Versterking van de systeembewaking wanneer er een indicatie is van een verhoogd risico. Dit zou de fysieke omgeving, personeel en dienstverlener moeten omvatten.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> = Début des exigences non ordonnées. Certianes sont toujours bien en ordre</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> = Exigences manquantes rajoutées</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> = Exigences mal placée et difficile à changer de place sans toucher le ref_id</t>
   </si>
   <si>
     <t>De fysieke omgeving van de faciliteit wordt bewaakt op potentiële informatie- /cyberbeveiligingsincidenten.</t>
@@ -6955,12 +6946,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -6971,17 +6956,23 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
@@ -6999,12 +6990,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDDBC351-7D88-493C-9B5D-79894BA0B34D}" name="Tableau3" displayName="Tableau3" ref="K1:M1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDDBC351-7D88-493C-9B5D-79894BA0B34D}" name="Tableau3" displayName="Tableau3" ref="K1:M1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="K1:M1048576" xr:uid="{CDDBC351-7D88-493C-9B5D-79894BA0B34D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{52685A48-3E2F-4BDE-AD86-0C7473E45D50}" name="name[nl]" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{EB38A65B-1968-426D-B37E-A7C196CA3A2A}" name="description[nl]" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{14D77745-A50F-4694-9737-292C8F18CB4D}" name="annotation[nl]" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{52685A48-3E2F-4BDE-AD86-0C7473E45D50}" name="name[nl]" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{EB38A65B-1968-426D-B37E-A7C196CA3A2A}" name="description[nl]" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{14D77745-A50F-4694-9737-292C8F18CB4D}" name="annotation[nl]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Style de tableau 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7297,8 +7288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B1651-6DC7-1E43-A5B6-8EF15B32842F}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7329,7 +7320,7 @@
         <v>1465</v>
       </c>
       <c r="B3" s="22">
-        <v>45676</v>
+        <v>45826</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7503,21 +7494,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="31"/>
-      <c r="B24" s="1" t="s">
-        <v>1885</v>
-      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="32"/>
-      <c r="B25" s="1" t="s">
-        <v>1886</v>
-      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="33"/>
-      <c r="B26" s="1" t="s">
-        <v>1887</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7530,8 +7512,8 @@
   <dimension ref="A1:M351"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L147" sqref="L147"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15371,7 +15353,7 @@
       </c>
       <c r="K260" s="19"/>
       <c r="L260" s="25" t="s">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="M260" s="19"/>
     </row>
@@ -15402,7 +15384,7 @@
       </c>
       <c r="K261" s="35"/>
       <c r="L261" s="36" t="s">
-        <v>1888</v>
+        <v>1885</v>
       </c>
       <c r="M261" s="35" t="s">
         <v>1510</v>
@@ -15435,10 +15417,10 @@
         <v>1281</v>
       </c>
       <c r="L262" s="8" t="s">
-        <v>1890</v>
+        <v>1887</v>
       </c>
       <c r="M262" s="8" t="s">
-        <v>1891</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="263" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15460,7 +15442,7 @@
       </c>
       <c r="K263" s="19"/>
       <c r="L263" s="25" t="s">
-        <v>1892</v>
+        <v>1889</v>
       </c>
       <c r="M263" s="19"/>
     </row>
@@ -15491,10 +15473,10 @@
         <v>1284</v>
       </c>
       <c r="L264" s="8" t="s">
-        <v>1893</v>
+        <v>1890</v>
       </c>
       <c r="M264" s="8" t="s">
-        <v>1894</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="265" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -15524,10 +15506,10 @@
         <v>1286</v>
       </c>
       <c r="L265" s="8" t="s">
-        <v>1895</v>
+        <v>1892</v>
       </c>
       <c r="M265" s="8" t="s">
-        <v>1896</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="266" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -15557,10 +15539,10 @@
         <v>1288</v>
       </c>
       <c r="L266" s="8" t="s">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="M266" s="8" t="s">
-        <v>1898</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="267" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -15582,7 +15564,7 @@
       </c>
       <c r="K267" s="19"/>
       <c r="L267" s="25" t="s">
-        <v>1899</v>
+        <v>1896</v>
       </c>
       <c r="M267" s="19"/>
     </row>
@@ -15613,10 +15595,10 @@
         <v>1290</v>
       </c>
       <c r="L268" s="8" t="s">
-        <v>1900</v>
+        <v>1897</v>
       </c>
       <c r="M268" s="8" t="s">
-        <v>1901</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="269" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -15646,7 +15628,7 @@
         <v>971</v>
       </c>
       <c r="L269" s="8" t="s">
-        <v>1902</v>
+        <v>1899</v>
       </c>
       <c r="M269" s="8" t="s">
         <v>1510</v>
@@ -15671,7 +15653,7 @@
       </c>
       <c r="K270" s="19"/>
       <c r="L270" s="25" t="s">
-        <v>1903</v>
+        <v>1900</v>
       </c>
       <c r="M270" s="19"/>
     </row>
@@ -15702,10 +15684,10 @@
         <v>1294</v>
       </c>
       <c r="L271" s="8" t="s">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="M271" s="8" t="s">
-        <v>1905</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="272" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15727,7 +15709,7 @@
       </c>
       <c r="K272" s="19"/>
       <c r="L272" s="25" t="s">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="M272" s="19"/>
     </row>
@@ -15758,10 +15740,10 @@
         <v>1297</v>
       </c>
       <c r="L273" s="8" t="s">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="M273" s="8" t="s">
-        <v>1908</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="274" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -15791,7 +15773,7 @@
         <v>971</v>
       </c>
       <c r="L274" s="8" t="s">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="M274" s="8" t="s">
         <v>1510</v>
@@ -15816,7 +15798,7 @@
       </c>
       <c r="K275" s="19"/>
       <c r="L275" s="25" t="s">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="M275" s="19"/>
     </row>
@@ -15847,10 +15829,10 @@
         <v>1301</v>
       </c>
       <c r="L276" s="8" t="s">
-        <v>1911</v>
+        <v>1908</v>
       </c>
       <c r="M276" s="8" t="s">
-        <v>1912</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="277" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -15880,7 +15862,7 @@
         <v>971</v>
       </c>
       <c r="L277" s="8" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
       <c r="M277" s="8" t="s">
         <v>1510</v>
@@ -15905,7 +15887,7 @@
       </c>
       <c r="K278" s="19"/>
       <c r="L278" s="25" t="s">
-        <v>1914</v>
+        <v>1911</v>
       </c>
       <c r="M278" s="19"/>
     </row>
@@ -15936,10 +15918,10 @@
         <v>1305</v>
       </c>
       <c r="L279" s="8" t="s">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="M279" s="8" t="s">
-        <v>1916</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="280" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -15969,7 +15951,7 @@
         <v>971</v>
       </c>
       <c r="L280" s="8" t="s">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="M280" s="8" t="s">
         <v>1510</v>
@@ -15999,10 +15981,10 @@
         <v>927</v>
       </c>
       <c r="K281" s="16" t="s">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="L281" s="24" t="s">
-        <v>1918</v>
+        <v>1915</v>
       </c>
       <c r="M281" s="16"/>
     </row>
@@ -16025,7 +16007,7 @@
       </c>
       <c r="K282" s="19"/>
       <c r="L282" s="25" t="s">
-        <v>1920</v>
+        <v>1917</v>
       </c>
       <c r="M282" s="19"/>
     </row>
@@ -16056,7 +16038,7 @@
         <v>971</v>
       </c>
       <c r="L283" s="8" t="s">
-        <v>1921</v>
+        <v>1918</v>
       </c>
       <c r="M283" s="8" t="s">
         <v>1510</v>
@@ -16081,7 +16063,7 @@
       </c>
       <c r="K284" s="19"/>
       <c r="L284" s="25" t="s">
-        <v>1922</v>
+        <v>1919</v>
       </c>
       <c r="M284" s="19"/>
     </row>
@@ -16112,10 +16094,10 @@
         <v>1313</v>
       </c>
       <c r="L285" s="8" t="s">
-        <v>1923</v>
+        <v>1920</v>
       </c>
       <c r="M285" s="8" t="s">
-        <v>1924</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="286" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16137,7 +16119,7 @@
       </c>
       <c r="K286" s="19"/>
       <c r="L286" s="25" t="s">
-        <v>1925</v>
+        <v>1922</v>
       </c>
       <c r="M286" s="19"/>
     </row>
@@ -16168,10 +16150,10 @@
         <v>1316</v>
       </c>
       <c r="L287" s="8" t="s">
-        <v>1926</v>
+        <v>1923</v>
       </c>
       <c r="M287" s="8" t="s">
-        <v>1927</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="288" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16193,7 +16175,7 @@
       </c>
       <c r="K288" s="19"/>
       <c r="L288" s="25" t="s">
-        <v>1928</v>
+        <v>1925</v>
       </c>
       <c r="M288" s="19"/>
     </row>
@@ -16224,10 +16206,10 @@
         <v>1319</v>
       </c>
       <c r="L289" s="8" t="s">
-        <v>1929</v>
+        <v>1926</v>
       </c>
       <c r="M289" s="8" t="s">
-        <v>1930</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="290" spans="1:13" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -16257,10 +16239,10 @@
         <v>1321</v>
       </c>
       <c r="L290" s="8" t="s">
-        <v>1931</v>
+        <v>1928</v>
       </c>
       <c r="M290" s="8" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="291" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16285,7 +16267,7 @@
         <v>927</v>
       </c>
       <c r="K291" s="12" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
       <c r="L291" s="23"/>
       <c r="M291" s="12"/>
@@ -16314,10 +16296,10 @@
         <v>927</v>
       </c>
       <c r="K292" s="16" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
       <c r="L292" s="24" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
       <c r="M292" s="16"/>
     </row>
@@ -16340,7 +16322,7 @@
       </c>
       <c r="K293" s="19"/>
       <c r="L293" s="25" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="M293" s="19"/>
     </row>
@@ -16371,10 +16353,10 @@
         <v>1327</v>
       </c>
       <c r="L294" s="8" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="M294" s="8" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="295" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16401,10 +16383,10 @@
         <v>927</v>
       </c>
       <c r="K295" s="16" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
       <c r="L295" s="24" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
       <c r="M295" s="16"/>
     </row>
@@ -16427,7 +16409,7 @@
       </c>
       <c r="K296" s="19"/>
       <c r="L296" s="25" t="s">
-        <v>1941</v>
+        <v>1938</v>
       </c>
       <c r="M296" s="19"/>
     </row>
@@ -16458,10 +16440,10 @@
         <v>1331</v>
       </c>
       <c r="L297" s="8" t="s">
-        <v>1942</v>
+        <v>1939</v>
       </c>
       <c r="M297" s="8" t="s">
-        <v>1943</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="298" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16483,7 +16465,7 @@
       </c>
       <c r="K298" s="19"/>
       <c r="L298" s="25" t="s">
-        <v>1944</v>
+        <v>1941</v>
       </c>
       <c r="M298" s="19"/>
     </row>
@@ -16514,10 +16496,10 @@
         <v>1334</v>
       </c>
       <c r="L299" s="8" t="s">
-        <v>1945</v>
+        <v>1942</v>
       </c>
       <c r="M299" s="8" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="300" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -16547,10 +16529,10 @@
         <v>1336</v>
       </c>
       <c r="L300" s="8" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
       <c r="M300" s="8" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="301" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16572,7 +16554,7 @@
       </c>
       <c r="K301" s="19"/>
       <c r="L301" s="25" t="s">
-        <v>1949</v>
+        <v>1946</v>
       </c>
       <c r="M301" s="19"/>
     </row>
@@ -16603,7 +16585,7 @@
         <v>971</v>
       </c>
       <c r="L302" s="8" t="s">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="M302" s="8" t="s">
         <v>1510</v>
@@ -16636,7 +16618,7 @@
         <v>971</v>
       </c>
       <c r="L303" s="8" t="s">
-        <v>1951</v>
+        <v>1948</v>
       </c>
       <c r="M303" s="8" t="s">
         <v>1510</v>
@@ -16661,7 +16643,7 @@
       </c>
       <c r="K304" s="19"/>
       <c r="L304" s="25" t="s">
-        <v>1952</v>
+        <v>1949</v>
       </c>
       <c r="M304" s="19"/>
     </row>
@@ -16692,10 +16674,10 @@
         <v>1342</v>
       </c>
       <c r="L305" s="8" t="s">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="M305" s="8" t="s">
-        <v>1954</v>
+        <v>1951</v>
       </c>
     </row>
     <row r="306" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -16717,7 +16699,7 @@
       </c>
       <c r="K306" s="19"/>
       <c r="L306" s="25" t="s">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="M306" s="19"/>
     </row>
@@ -16748,7 +16730,7 @@
         <v>971</v>
       </c>
       <c r="L307" s="8" t="s">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="M307" s="8" t="s">
         <v>1510</v>
@@ -16781,7 +16763,7 @@
         <v>1345</v>
       </c>
       <c r="L308" s="24" t="s">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="M308" s="16"/>
     </row>
@@ -16804,7 +16786,7 @@
       </c>
       <c r="K309" s="19"/>
       <c r="L309" s="25" t="s">
-        <v>1958</v>
+        <v>1955</v>
       </c>
       <c r="M309" s="19"/>
     </row>
@@ -16835,7 +16817,7 @@
         <v>971</v>
       </c>
       <c r="L310" s="8" t="s">
-        <v>1959</v>
+        <v>1956</v>
       </c>
       <c r="M310" s="8" t="s">
         <v>1510</v>
@@ -16868,7 +16850,7 @@
         <v>971</v>
       </c>
       <c r="L311" s="8" t="s">
-        <v>1960</v>
+        <v>1957</v>
       </c>
       <c r="M311" s="8" t="s">
         <v>1510</v>
@@ -16893,7 +16875,7 @@
       </c>
       <c r="K312" s="19"/>
       <c r="L312" s="25" t="s">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="M312" s="19"/>
     </row>
@@ -16924,10 +16906,10 @@
         <v>1352</v>
       </c>
       <c r="L313" s="8" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="M313" s="8" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="314" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -16957,10 +16939,10 @@
         <v>1354</v>
       </c>
       <c r="L314" s="8" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="M314" s="8" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="315" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -16982,7 +16964,7 @@
       </c>
       <c r="K315" s="19"/>
       <c r="L315" s="25" t="s">
-        <v>1966</v>
+        <v>1963</v>
       </c>
       <c r="M315" s="19"/>
     </row>
@@ -17013,7 +16995,7 @@
         <v>971</v>
       </c>
       <c r="L316" s="8" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="M316" s="8" t="s">
         <v>1510</v>
@@ -17046,10 +17028,10 @@
         <v>1358</v>
       </c>
       <c r="L317" s="8" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="M317" s="8" t="s">
-        <v>1969</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="318" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -17071,7 +17053,7 @@
       </c>
       <c r="K318" s="19"/>
       <c r="L318" s="25" t="s">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="M318" s="19"/>
     </row>
@@ -17102,10 +17084,10 @@
         <v>1361</v>
       </c>
       <c r="L319" s="8" t="s">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="M319" s="8" t="s">
-        <v>1972</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="320" spans="1:13" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -17127,7 +17109,7 @@
       </c>
       <c r="K320" s="19"/>
       <c r="L320" s="25" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="M320" s="19"/>
     </row>
@@ -17158,7 +17140,7 @@
         <v>971</v>
       </c>
       <c r="L321" s="8" t="s">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="M321" s="8" t="s">
         <v>1510</v>
@@ -17191,7 +17173,7 @@
         <v>971</v>
       </c>
       <c r="L322" s="8" t="s">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="M322" s="8" t="s">
         <v>1510</v>
@@ -17221,10 +17203,10 @@
         <v>927</v>
       </c>
       <c r="K323" s="16" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="L323" s="24" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="M323" s="16"/>
     </row>
@@ -17247,7 +17229,7 @@
       </c>
       <c r="K324" s="19"/>
       <c r="L324" s="25" t="s">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="M324" s="19"/>
     </row>
@@ -17283,7 +17265,7 @@
       <c r="J326" s="19"/>
       <c r="K326" s="19"/>
       <c r="L326" s="25" t="s">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="M326" s="19"/>
     </row>
@@ -17319,7 +17301,7 @@
       <c r="J328" s="19"/>
       <c r="K328" s="19"/>
       <c r="L328" s="25" t="s">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="M328" s="19"/>
     </row>
@@ -17350,10 +17332,10 @@
         <v>1368</v>
       </c>
       <c r="L329" s="8" t="s">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="M329" s="8" t="s">
-        <v>1981</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="330" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -17380,10 +17362,10 @@
         <v>927</v>
       </c>
       <c r="K330" s="16" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="L330" s="24" t="s">
-        <v>1982</v>
+        <v>1979</v>
       </c>
       <c r="M330" s="16"/>
     </row>
@@ -17406,7 +17388,7 @@
       </c>
       <c r="K331" s="19"/>
       <c r="L331" s="25" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="M331" s="19"/>
     </row>
@@ -17437,10 +17419,10 @@
         <v>1372</v>
       </c>
       <c r="L332" s="8" t="s">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="M332" s="8" t="s">
-        <v>1986</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="333" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -17470,7 +17452,7 @@
         <v>971</v>
       </c>
       <c r="L333" s="8" t="s">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="M333" s="8" t="s">
         <v>1510</v>
@@ -17495,7 +17477,7 @@
       </c>
       <c r="K334" s="19"/>
       <c r="L334" s="25" t="s">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="M334" s="19"/>
     </row>
@@ -17526,10 +17508,10 @@
         <v>1375</v>
       </c>
       <c r="L335" s="8" t="s">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="M335" s="8" t="s">
-        <v>1990</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="336" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17554,7 +17536,7 @@
         <v>927</v>
       </c>
       <c r="K336" s="12" t="s">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="L336" s="23"/>
       <c r="M336" s="12"/>
@@ -17583,10 +17565,10 @@
         <v>927</v>
       </c>
       <c r="K337" s="16" t="s">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="L337" s="24" t="s">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="M337" s="16"/>
     </row>
@@ -17609,7 +17591,7 @@
       </c>
       <c r="K338" s="19"/>
       <c r="L338" s="25" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="M338" s="19"/>
     </row>
@@ -17637,13 +17619,13 @@
         <v>1380</v>
       </c>
       <c r="J339" s="8" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="L339" s="8" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="M339" s="8" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -17673,7 +17655,7 @@
         <v>971</v>
       </c>
       <c r="L340" s="8" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="M340" s="8" t="s">
         <v>1510</v>
@@ -17703,10 +17685,10 @@
         <v>927</v>
       </c>
       <c r="K341" s="16" t="s">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="L341" s="24" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="M341" s="16"/>
     </row>
@@ -17729,7 +17711,7 @@
       </c>
       <c r="K342" s="19"/>
       <c r="L342" s="25" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="M342" s="19"/>
     </row>
@@ -17760,7 +17742,7 @@
         <v>971</v>
       </c>
       <c r="L343" s="8" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="M343" s="8" t="s">
         <v>1510</v>
@@ -17790,10 +17772,10 @@
         <v>927</v>
       </c>
       <c r="K344" s="16" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
       <c r="L344" s="24" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="M344" s="16"/>
     </row>
@@ -17816,7 +17798,7 @@
       </c>
       <c r="K345" s="19"/>
       <c r="L345" s="25" t="s">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="M345" s="19"/>
     </row>
@@ -17847,10 +17829,10 @@
         <v>1387</v>
       </c>
       <c r="L346" s="8" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="M346" s="8" t="s">
-        <v>2004</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -17880,10 +17862,10 @@
         <v>1389</v>
       </c>
       <c r="L347" s="8" t="s">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="M347" s="8" t="s">
-        <v>2006</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="348" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -17905,7 +17887,7 @@
       </c>
       <c r="K348" s="19"/>
       <c r="L348" s="25" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="M348" s="19"/>
     </row>
@@ -17936,10 +17918,10 @@
         <v>1392</v>
       </c>
       <c r="L349" s="8" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="M349" s="8" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="350" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -17961,7 +17943,7 @@
       </c>
       <c r="K350" s="19"/>
       <c r="L350" s="25" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="M350" s="19"/>
     </row>
@@ -17992,10 +17974,10 @@
         <v>1395</v>
       </c>
       <c r="L351" s="8" t="s">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="M351" s="8" t="s">
-        <v>2012</v>
+        <v>2009</v>
       </c>
     </row>
   </sheetData>
@@ -18012,7 +17994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8EE66F-5BF1-6F47-9F88-8D8C53839AC6}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add missing translations for Dutch + Small Fixes
Added missing translations for "library_content", "scores" and "implementation_groups" in Dutch in Excel and YAML files.
Fixed a few French translations in the "library_content" section.
</commit_message>
<xml_diff>
--- a/tools/excel/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/excel/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\ccb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C34A257-2480-4D4F-8E4A-413AD45D6DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87B3467-4ACA-4F2A-8E06-954A8745E8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="312" yWindow="48" windowWidth="21264" windowHeight="12912" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2807" uniqueCount="2011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2841" uniqueCount="2039">
   <si>
     <t>assessable</t>
   </si>
@@ -4860,14 +4860,6 @@
   </si>
   <si>
     <t>CCB CyberFondamentaux - 2023-03-01</t>
-  </si>
-  <si>
-    <t>Centre For Cybersecurity Belgium - CyberFondamentaux</t>
-  </si>
-  <si>
-    <t>Centre For Cybersecurity Belgium - CyberFondamentaux
-With content from CyFun Self-Assessment tool V2024-11-05
-https://ccb.belgium.be</t>
   </si>
   <si>
     <t>Un processus formel existe et est mis en œuvre.
@@ -6708,12 +6700,108 @@
   <si>
     <t>[KERNMAATREGEL] De organisatie moet processen en procedures voor het beheer van kwetsbaarheden toepassen die het verwerken, analyseren en verhelpen van kwetsbaarheden uit interne en externe bronnen omvatten.</t>
   </si>
+  <si>
+    <t>library_name[nl]</t>
+  </si>
+  <si>
+    <t>library_description[nl]</t>
+  </si>
+  <si>
+    <t>framework_name[nl]</t>
+  </si>
+  <si>
+    <t>framework_description[nl]</t>
+  </si>
+  <si>
+    <t>Centre pour la Cybersécurité Belgique - CyberFondamentaux</t>
+  </si>
+  <si>
+    <t>Centrum voor Cybersecurity België - CyberFundamentals</t>
+  </si>
+  <si>
+    <t>Centre pour la Cybersécurité Belgique- CyberFondamentaux
+Avec le contenu de CyFun Self-Assessment tool V2024-11-05
+https://ccb.belgium.be</t>
+  </si>
+  <si>
+    <t>Centrum voor Cybersecurity België - CyberFondamentaux
+Met inhoud van CyFun Self-Assessment tool V2024-11-05
+https://ccb.belgium.be</t>
+  </si>
+  <si>
+    <t>basis</t>
+  </si>
+  <si>
+    <t>belangrijk</t>
+  </si>
+  <si>
+    <t>essentieel</t>
+  </si>
+  <si>
+    <t>basis - kernmaatregel</t>
+  </si>
+  <si>
+    <t>belangrijk - kernmaatregel</t>
+  </si>
+  <si>
+    <t>essentieel - kernmaatregel</t>
+  </si>
+  <si>
+    <t>description_doc[nl]</t>
+  </si>
+  <si>
+    <t>Initiële</t>
+  </si>
+  <si>
+    <t>Herhaalbaar</t>
+  </si>
+  <si>
+    <t>Gedefinieerd</t>
+  </si>
+  <si>
+    <t>Beheerd</t>
+  </si>
+  <si>
+    <t>Geoptimaliseerd</t>
+  </si>
+  <si>
+    <t>Er bestaat geen standaardproces.</t>
+  </si>
+  <si>
+    <t>Er bestaat een ad-hocproces dat informeel wordt uitgevoerd.</t>
+  </si>
+  <si>
+    <t>Formeel proces bestaat en wordt geïmplementeerd. Bewijs beschikbaar voor de meeste activiteiten. Minder dan 10% procesuitzonderingen.</t>
+  </si>
+  <si>
+    <t>Formeel proces bestaat en wordt geïmplementeerd. Voor alle activiteiten is bewijsmateriaal beschikbaar. Gedetailleerde metriek van het proces wordt vastgelegd en gerapporteerd.
+Minimale doelstelling voor metriek is vastgesteld. Minder dan 5% van de procesuitzonderingen.</t>
+  </si>
+  <si>
+    <t>Formeel proces bestaat en wordt geïmplementeerd. Voor alle activiteiten is bewijsmateriaal beschikbaar. Gedetailleerde metriek van het proces wordt vastgelegd en gerapporteerd..
+Minimale doelstelling voor metriek is vastgesteld en wordt voortdurend verbeterd. Minder dan 1% van de procesuitzonderingen.</t>
+  </si>
+  <si>
+    <t>Geen procesdocumentatie of niet formeel goedgekeurd door het management.</t>
+  </si>
+  <si>
+    <t>Er bestaat formeel goedgekeurde Procesdocumentatie, maar deze is de afgelopen 2 jaar niet herzien.</t>
+  </si>
+  <si>
+    <t>Er bestaat formeel goedgekeurde procesdocumentatie en uitzonderingen worden gedocumenteerd en goedgekeurd. Gedocumenteerde en goedgekeurde uitzonderingen &lt; 5% van de tijd.</t>
+  </si>
+  <si>
+    <t>Er bestaat formeel goedgekeurde procesdocumentatie en uitzonderingen worden gedocumenteerd en goedgekeurd. Gedocumenteerde en goedgekeurde uitzonderingen &lt; 3% van de tijd.</t>
+  </si>
+  <si>
+    <t>Er bestaat formeel goedgekeurde procesdocumentatie en uitzonderingen worden gedocumenteerd en goedgekeurd. Gedocumenteerde en goedgekeurde uitzonderingen &lt; 0,5% van de tijd.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6747,15 +6835,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6783,12 +6864,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6839,7 +6914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -6919,16 +6994,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7286,15 +7359,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B1651-6DC7-1E43-A5B6-8EF15B32842F}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="111.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -7473,7 +7546,7 @@
         <v>1469</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>1474</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -7489,17 +7562,40 @@
         <v>1471</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1473</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="31"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
+      <c r="A24" t="s">
+        <v>2009</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>2016</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="33"/>
+      <c r="A26" t="s">
+        <v>2011</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>2014</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7511,7 +7607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
@@ -7564,14 +7660,14 @@
       <c r="J1" s="6" t="s">
         <v>1398</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="35" t="s">
+        <v>1487</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>1488</v>
+      </c>
+      <c r="M1" s="35" t="s">
         <v>1489</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>1490</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>1491</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -7596,7 +7692,7 @@
         <v>927</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="12"/>
@@ -7625,10 +7721,10 @@
         <v>927</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="M3" s="16"/>
     </row>
@@ -7651,7 +7747,7 @@
       </c>
       <c r="K4" s="19"/>
       <c r="L4" s="25" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="M4" s="19"/>
     </row>
@@ -7682,10 +7778,10 @@
         <v>932</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="M5" s="26" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
@@ -7715,10 +7811,10 @@
         <v>934</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -7748,10 +7844,10 @@
         <v>936</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -7781,10 +7877,10 @@
         <v>938</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7806,7 +7902,7 @@
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="25" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="M9" s="19"/>
     </row>
@@ -7837,10 +7933,10 @@
         <v>941</v>
       </c>
       <c r="L10" s="26" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -7870,10 +7966,10 @@
         <v>943</v>
       </c>
       <c r="L11" s="26" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -7903,10 +7999,10 @@
         <v>971</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -7936,10 +8032,10 @@
         <v>946</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -7969,10 +8065,10 @@
         <v>938</v>
       </c>
       <c r="L14" s="26" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7994,7 +8090,7 @@
       </c>
       <c r="K15" s="19"/>
       <c r="L15" s="25" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="M15" s="19"/>
     </row>
@@ -8025,10 +8121,10 @@
         <v>950</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
@@ -8058,10 +8154,10 @@
         <v>952</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
@@ -8091,10 +8187,10 @@
         <v>1412</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -8116,7 +8212,7 @@
       </c>
       <c r="K19" s="19"/>
       <c r="L19" s="25" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="M19" s="19"/>
     </row>
@@ -8147,10 +8243,10 @@
         <v>956</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -8180,10 +8276,10 @@
         <v>958</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="22" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8205,7 +8301,7 @@
       </c>
       <c r="K22" s="19"/>
       <c r="L22" s="25" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="M22" s="19"/>
     </row>
@@ -8236,10 +8332,10 @@
         <v>1411</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8261,7 +8357,7 @@
       </c>
       <c r="K24" s="19"/>
       <c r="L24" s="25" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="M24" s="19"/>
     </row>
@@ -8292,10 +8388,10 @@
         <v>962</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -8325,10 +8421,10 @@
         <v>964</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -8355,10 +8451,10 @@
         <v>927</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="M27" s="16"/>
     </row>
@@ -8381,7 +8477,7 @@
       </c>
       <c r="K28" s="19"/>
       <c r="L28" s="25" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="M28" s="19"/>
     </row>
@@ -8412,10 +8508,10 @@
         <v>969</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -8445,10 +8541,10 @@
         <v>971</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8470,7 +8566,7 @@
       </c>
       <c r="K31" s="19"/>
       <c r="L31" s="25" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="M31" s="19"/>
     </row>
@@ -8501,10 +8597,10 @@
         <v>974</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -8524,7 +8620,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
       <c r="L33" s="25" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="M33" s="19"/>
     </row>
@@ -8555,10 +8651,10 @@
         <v>1399</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8580,7 +8676,7 @@
       </c>
       <c r="K35" s="19"/>
       <c r="L35" s="25" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="M35" s="19"/>
     </row>
@@ -8611,10 +8707,10 @@
         <v>979</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -8636,7 +8732,7 @@
       </c>
       <c r="K37" s="19"/>
       <c r="L37" s="25" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="M37" s="19"/>
     </row>
@@ -8667,10 +8763,10 @@
         <v>982</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="216" x14ac:dyDescent="0.3">
@@ -8700,10 +8796,10 @@
         <v>984</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -8733,10 +8829,10 @@
         <v>986</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="41" spans="1:13" s="13" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -8763,10 +8859,10 @@
         <v>927</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="L41" s="24" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="M41" s="16"/>
     </row>
@@ -8789,7 +8885,7 @@
       </c>
       <c r="K42" s="19"/>
       <c r="L42" s="25" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="M42" s="19"/>
     </row>
@@ -8820,10 +8916,10 @@
         <v>991</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -8853,10 +8949,10 @@
         <v>993</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="45" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -8878,7 +8974,7 @@
       </c>
       <c r="K45" s="19"/>
       <c r="L45" s="25" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="M45" s="19"/>
     </row>
@@ -8909,10 +9005,10 @@
         <v>996</v>
       </c>
       <c r="L46" s="8" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -8942,10 +9038,10 @@
         <v>998</v>
       </c>
       <c r="L47" s="8" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="48" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8967,7 +9063,7 @@
       </c>
       <c r="K48" s="19"/>
       <c r="L48" s="25" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="M48" s="19"/>
     </row>
@@ -8998,10 +9094,10 @@
         <v>1001</v>
       </c>
       <c r="L49" s="8" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -9031,10 +9127,10 @@
         <v>1003</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="51" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -9061,10 +9157,10 @@
         <v>927</v>
       </c>
       <c r="K51" s="16" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="L51" s="24" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="M51" s="16"/>
     </row>
@@ -9087,7 +9183,7 @@
       </c>
       <c r="K52" s="19"/>
       <c r="L52" s="25" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="M52" s="19"/>
     </row>
@@ -9118,10 +9214,10 @@
         <v>1008</v>
       </c>
       <c r="L53" s="8" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="M53" s="8" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -9151,10 +9247,10 @@
         <v>1010</v>
       </c>
       <c r="L54" s="8" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="M54" s="8" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -9184,10 +9280,10 @@
         <v>1012</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="56" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9209,7 +9305,7 @@
       </c>
       <c r="K56" s="19"/>
       <c r="L56" s="25" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="M56" s="19"/>
     </row>
@@ -9240,10 +9336,10 @@
         <v>1015</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -9273,10 +9369,10 @@
         <v>971</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="M58" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="59" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9298,7 +9394,7 @@
       </c>
       <c r="K59" s="19"/>
       <c r="L59" s="25" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="M59" s="19"/>
     </row>
@@ -9329,10 +9425,10 @@
         <v>1019</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="M60" s="8" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -9362,10 +9458,10 @@
         <v>1021</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="M61" s="8" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -9395,10 +9491,10 @@
         <v>971</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="M62" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="63" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9420,7 +9516,7 @@
       </c>
       <c r="K63" s="19"/>
       <c r="L63" s="25" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="M63" s="19"/>
     </row>
@@ -9451,10 +9547,10 @@
         <v>1025</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="M64" s="8" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="65" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -9481,10 +9577,10 @@
         <v>927</v>
       </c>
       <c r="K65" s="16" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="L65" s="24" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="M65" s="16"/>
     </row>
@@ -9507,7 +9603,7 @@
       </c>
       <c r="K66" s="19"/>
       <c r="L66" s="25" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="M66" s="19"/>
     </row>
@@ -9538,10 +9634,10 @@
         <v>1030</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="M67" s="8" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="68" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -9563,7 +9659,7 @@
       </c>
       <c r="K68" s="19"/>
       <c r="L68" s="25" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="M68" s="19"/>
     </row>
@@ -9594,10 +9690,10 @@
         <v>1033</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="70" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -9619,7 +9715,7 @@
       </c>
       <c r="K70" s="19"/>
       <c r="L70" s="25" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="M70" s="19"/>
     </row>
@@ -9650,10 +9746,10 @@
         <v>971</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="M71" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="72" spans="1:13" s="13" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -9680,10 +9776,10 @@
         <v>927</v>
       </c>
       <c r="K72" s="16" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="L72" s="24" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="M72" s="16"/>
     </row>
@@ -9706,7 +9802,7 @@
       </c>
       <c r="K73" s="19"/>
       <c r="L73" s="25" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="M73" s="19"/>
     </row>
@@ -9737,10 +9833,10 @@
         <v>971</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="M74" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="75" spans="1:13" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -9762,7 +9858,7 @@
       </c>
       <c r="K75" s="19"/>
       <c r="L75" s="25" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="M75" s="19"/>
     </row>
@@ -9793,10 +9889,10 @@
         <v>1042</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="M76" s="8" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -9826,10 +9922,10 @@
         <v>1044</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="78" spans="1:13" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -9851,7 +9947,7 @@
       </c>
       <c r="K78" s="19"/>
       <c r="L78" s="25" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="M78" s="19"/>
     </row>
@@ -9882,10 +9978,10 @@
         <v>1047</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="M79" s="8" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
@@ -9915,10 +10011,10 @@
         <v>1048</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -9948,10 +10044,10 @@
         <v>971</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="M81" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -9973,7 +10069,7 @@
       </c>
       <c r="K82" s="19"/>
       <c r="L82" s="25" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="M82" s="19"/>
     </row>
@@ -10004,10 +10100,10 @@
         <v>1051</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="M83" s="8" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -10037,10 +10133,10 @@
         <v>1053</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="M84" s="8" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="85" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -10062,7 +10158,7 @@
       </c>
       <c r="K85" s="19"/>
       <c r="L85" s="25" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="M85" s="19"/>
     </row>
@@ -10093,10 +10189,10 @@
         <v>1051</v>
       </c>
       <c r="L86" s="8" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="M86" s="8" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -10126,10 +10222,10 @@
         <v>971</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="M87" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="88" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -10152,7 +10248,7 @@
         <v>927</v>
       </c>
       <c r="K88" s="12" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="L88" s="23"/>
       <c r="M88" s="12"/>
@@ -10181,10 +10277,10 @@
         <v>927</v>
       </c>
       <c r="K89" s="16" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="L89" s="24" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="M89" s="16"/>
     </row>
@@ -10207,7 +10303,7 @@
       </c>
       <c r="K90" s="19"/>
       <c r="L90" s="25" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="M90" s="19"/>
     </row>
@@ -10238,10 +10334,10 @@
         <v>1061</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="M91" s="8" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="216" x14ac:dyDescent="0.3">
@@ -10271,10 +10367,10 @@
         <v>1063</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="M92" s="8" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -10304,10 +10400,10 @@
         <v>1065</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="M93" s="8" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -10337,10 +10433,10 @@
         <v>1067</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="M94" s="8" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -10370,10 +10466,10 @@
         <v>1069</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="M95" s="8" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="96" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -10395,7 +10491,7 @@
       </c>
       <c r="K96" s="19"/>
       <c r="L96" s="25" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="M96" s="19"/>
     </row>
@@ -10426,10 +10522,10 @@
         <v>1410</v>
       </c>
       <c r="L97" s="8" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="M97" s="8" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
@@ -10459,10 +10555,10 @@
         <v>1409</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="M98" s="8" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -10492,10 +10588,10 @@
         <v>1074</v>
       </c>
       <c r="L99" s="8" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="M99" s="8" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -10525,10 +10621,10 @@
         <v>1076</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="M100" s="8" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="101" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -10550,7 +10646,7 @@
       </c>
       <c r="K101" s="19"/>
       <c r="L101" s="25" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="M101" s="19"/>
     </row>
@@ -10581,10 +10677,10 @@
         <v>1079</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="M102" s="8" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="103" spans="1:13" s="27" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -10614,10 +10710,10 @@
       </c>
       <c r="K103" s="29"/>
       <c r="L103" s="30" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="M103" s="29" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="230.4" x14ac:dyDescent="0.3">
@@ -10647,10 +10743,10 @@
         <v>1081</v>
       </c>
       <c r="L104" s="26" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="M104" s="8" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -10680,10 +10776,10 @@
         <v>1083</v>
       </c>
       <c r="L105" s="8" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="M105" s="8" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -10713,10 +10809,10 @@
         <v>1085</v>
       </c>
       <c r="L106" s="8" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="M106" s="8" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="107" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -10738,7 +10834,7 @@
       </c>
       <c r="K107" s="19"/>
       <c r="L107" s="25" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="M107" s="19"/>
     </row>
@@ -10769,10 +10865,10 @@
         <v>1087</v>
       </c>
       <c r="L108" s="8" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="M108" s="8" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -10802,10 +10898,10 @@
         <v>1088</v>
       </c>
       <c r="L109" s="8" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="M109" s="8" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="244.8" x14ac:dyDescent="0.3">
@@ -10835,10 +10931,10 @@
         <v>1089</v>
       </c>
       <c r="L110" s="8" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="M110" s="8" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="144" x14ac:dyDescent="0.3">
@@ -10868,10 +10964,10 @@
         <v>1400</v>
       </c>
       <c r="L111" s="8" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="M111" s="8" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -10901,10 +10997,10 @@
         <v>1091</v>
       </c>
       <c r="L112" s="8" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="M112" s="8" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="158.4" x14ac:dyDescent="0.3">
@@ -10934,10 +11030,10 @@
         <v>1093</v>
       </c>
       <c r="L113" s="8" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="M113" s="8" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -10967,10 +11063,10 @@
         <v>971</v>
       </c>
       <c r="L114" s="26" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="M114" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -11000,10 +11096,10 @@
         <v>1096</v>
       </c>
       <c r="L115" s="8" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="M115" s="8" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="116" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -11033,10 +11129,10 @@
         <v>971</v>
       </c>
       <c r="L116" s="8" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="M116" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="117" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11058,7 +11154,7 @@
       </c>
       <c r="K117" s="19"/>
       <c r="L117" s="25" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="M117" s="19"/>
     </row>
@@ -11089,10 +11185,10 @@
         <v>1408</v>
       </c>
       <c r="L118" s="8" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="M118" s="8" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="119" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -11122,10 +11218,10 @@
         <v>1098</v>
       </c>
       <c r="L119" s="8" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="M119" s="8" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="120" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -11149,16 +11245,16 @@
       </c>
       <c r="H120"/>
       <c r="I120" s="8" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="J120" s="8" t="s">
         <v>1099</v>
       </c>
       <c r="L120" s="8" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="M120" s="8" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="121" spans="1:13" ht="259.2" x14ac:dyDescent="0.3">
@@ -11188,10 +11284,10 @@
         <v>1100</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="122" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -11221,10 +11317,10 @@
         <v>971</v>
       </c>
       <c r="L122" s="8" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="M122" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="123" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -11254,10 +11350,10 @@
         <v>971</v>
       </c>
       <c r="L123" s="26" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="M123" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="124" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11279,7 +11375,7 @@
       </c>
       <c r="K124" s="19"/>
       <c r="L124" s="25" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="M124" s="19"/>
     </row>
@@ -11310,10 +11406,10 @@
         <v>971</v>
       </c>
       <c r="L125" s="8" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="M125" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -11343,10 +11439,10 @@
         <v>971</v>
       </c>
       <c r="L126" s="8" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="M126" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="127" spans="1:13" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -11368,7 +11464,7 @@
       </c>
       <c r="K127" s="19"/>
       <c r="L127" s="25" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="M127" s="19"/>
     </row>
@@ -11398,10 +11494,10 @@
         <v>1106</v>
       </c>
       <c r="L128" s="8" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="M128" s="8" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="129" spans="1:13" s="13" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -11428,10 +11524,10 @@
         <v>927</v>
       </c>
       <c r="K129" s="16" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="L129" s="24" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="M129" s="16"/>
     </row>
@@ -11454,7 +11550,7 @@
       </c>
       <c r="K130" s="19"/>
       <c r="L130" s="25" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="M130" s="19"/>
     </row>
@@ -11485,10 +11581,10 @@
         <v>1111</v>
       </c>
       <c r="L131" s="8" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="M131" s="8" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="132" spans="1:13" ht="409.6" x14ac:dyDescent="0.3">
@@ -11518,10 +11614,10 @@
         <v>1407</v>
       </c>
       <c r="L132" s="8" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="M132" s="8" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="133" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -11551,10 +11647,10 @@
         <v>971</v>
       </c>
       <c r="L133" s="8" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="M133" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="134" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11576,7 +11672,7 @@
       </c>
       <c r="K134" s="19"/>
       <c r="L134" s="25" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="M134" s="19"/>
     </row>
@@ -11607,10 +11703,10 @@
         <v>971</v>
       </c>
       <c r="L135" s="8" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="M135" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="136" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -11632,7 +11728,7 @@
       </c>
       <c r="K136" s="19"/>
       <c r="L136" s="25" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="M136" s="19"/>
     </row>
@@ -11663,10 +11759,10 @@
         <v>1118</v>
       </c>
       <c r="L137" s="8" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="M137" s="8" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="138" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -11696,10 +11792,10 @@
         <v>1120</v>
       </c>
       <c r="L138" s="8" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="M138" s="8" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="139" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -11729,10 +11825,10 @@
         <v>1122</v>
       </c>
       <c r="L139" s="8" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="M139" s="8" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="140" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -11762,10 +11858,10 @@
         <v>1122</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="141" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11787,7 +11883,7 @@
       </c>
       <c r="K141" s="19"/>
       <c r="L141" s="25" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="M141" s="19"/>
     </row>
@@ -11818,10 +11914,10 @@
         <v>1126</v>
       </c>
       <c r="L142" s="8" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="M142" s="8" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="143" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -11843,7 +11939,7 @@
       </c>
       <c r="K143" s="19"/>
       <c r="L143" s="25" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="M143" s="19"/>
     </row>
@@ -11873,10 +11969,10 @@
         <v>971</v>
       </c>
       <c r="L144" s="8" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="M144" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="145" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -11903,10 +11999,10 @@
         <v>927</v>
       </c>
       <c r="K145" s="24" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="L145" s="16" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="M145" s="15"/>
     </row>
@@ -11929,9 +12025,9 @@
       </c>
       <c r="K146" s="25"/>
       <c r="L146" s="19" t="s">
-        <v>1721</v>
-      </c>
-      <c r="M146" s="39"/>
+        <v>1719</v>
+      </c>
+      <c r="M146" s="37"/>
     </row>
     <row r="147" spans="1:13" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
@@ -11960,10 +12056,10 @@
         <v>1133</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="M147" s="8" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="148" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -11985,7 +12081,7 @@
       </c>
       <c r="K148" s="19"/>
       <c r="L148" s="25" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
       <c r="M148" s="19"/>
     </row>
@@ -12016,10 +12112,10 @@
         <v>1136</v>
       </c>
       <c r="L149" s="8" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="M149" s="8" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="150" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -12041,7 +12137,7 @@
       </c>
       <c r="K150" s="19"/>
       <c r="L150" s="25" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="M150" s="19"/>
     </row>
@@ -12072,10 +12168,10 @@
         <v>1139</v>
       </c>
       <c r="L151" s="8" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="M151" s="8" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="152" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -12105,10 +12201,10 @@
         <v>1141</v>
       </c>
       <c r="L152" s="8" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
       <c r="M152" s="8" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="153" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -12138,10 +12234,10 @@
         <v>1143</v>
       </c>
       <c r="L153" s="8" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="M153" s="8" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="154" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -12171,10 +12267,10 @@
         <v>1145</v>
       </c>
       <c r="L154" s="8" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="M154" s="8" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="155" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12196,7 +12292,7 @@
       </c>
       <c r="K155" s="19"/>
       <c r="L155" s="25" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="M155" s="19"/>
     </row>
@@ -12227,10 +12323,10 @@
         <v>971</v>
       </c>
       <c r="L156" s="8" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="M156" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="157" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -12260,10 +12356,10 @@
         <v>1149</v>
       </c>
       <c r="L157" s="8" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="M157" s="8" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="158" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -12293,10 +12389,10 @@
         <v>971</v>
       </c>
       <c r="L158" s="8" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="M158" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="159" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12318,7 +12414,7 @@
       </c>
       <c r="K159" s="19"/>
       <c r="L159" s="25" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
       <c r="M159" s="19"/>
     </row>
@@ -12349,10 +12445,10 @@
         <v>1152</v>
       </c>
       <c r="L160" s="8" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
       <c r="M160" s="8" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -12374,7 +12470,7 @@
       </c>
       <c r="K161" s="19"/>
       <c r="L161" s="25" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
       <c r="M161" s="19"/>
     </row>
@@ -12405,10 +12501,10 @@
         <v>1155</v>
       </c>
       <c r="L162" s="8" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="M162" s="8" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="163" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -12438,10 +12534,10 @@
         <v>971</v>
       </c>
       <c r="L163" s="8" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="M163" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="164" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -12471,10 +12567,10 @@
         <v>971</v>
       </c>
       <c r="L164" s="8" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="M164" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -12496,7 +12592,7 @@
       </c>
       <c r="K165" s="19"/>
       <c r="L165" s="25" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="M165" s="19"/>
     </row>
@@ -12527,10 +12623,10 @@
         <v>1160</v>
       </c>
       <c r="L166" s="8" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="M166" s="8" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="167" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12552,7 +12648,7 @@
       </c>
       <c r="K167" s="19"/>
       <c r="L167" s="25" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="M167" s="19"/>
     </row>
@@ -12583,10 +12679,10 @@
         <v>1155</v>
       </c>
       <c r="L168" s="8" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="M168" s="8" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -12615,10 +12711,10 @@
         <v>971</v>
       </c>
       <c r="L169" s="8" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="M169" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="170" spans="1:13" s="13" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -12645,10 +12741,10 @@
         <v>927</v>
       </c>
       <c r="K170" s="16" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="L170" s="24" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="M170" s="16"/>
     </row>
@@ -12671,7 +12767,7 @@
       </c>
       <c r="K171" s="19"/>
       <c r="L171" s="25" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="M171" s="19"/>
     </row>
@@ -12702,10 +12798,10 @@
         <v>1167</v>
       </c>
       <c r="L172" s="8" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="M172" s="8" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="173" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -12735,10 +12831,10 @@
         <v>1169</v>
       </c>
       <c r="L173" s="8" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="M173" s="8" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="174" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12760,7 +12856,7 @@
       </c>
       <c r="K174" s="19"/>
       <c r="L174" s="25" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="M174" s="19"/>
     </row>
@@ -12791,10 +12887,10 @@
         <v>1406</v>
       </c>
       <c r="L175" s="8" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="M175" s="8" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="176" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -12824,10 +12920,10 @@
         <v>1173</v>
       </c>
       <c r="L176" s="8" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="M176" s="8" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="177" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12849,7 +12945,7 @@
       </c>
       <c r="K177" s="19"/>
       <c r="L177" s="25" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="M177" s="19"/>
     </row>
@@ -12880,10 +12976,10 @@
         <v>971</v>
       </c>
       <c r="L178" s="8" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
       <c r="M178" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="179" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -12913,10 +13009,10 @@
         <v>971</v>
       </c>
       <c r="L179" s="8" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="M179" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="180" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -12938,7 +13034,7 @@
       </c>
       <c r="K180" s="19"/>
       <c r="L180" s="25" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="M180" s="19"/>
     </row>
@@ -12969,10 +13065,10 @@
         <v>1178</v>
       </c>
       <c r="L181" s="8" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="M181" s="8" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="182" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -13002,10 +13098,10 @@
         <v>1180</v>
       </c>
       <c r="L182" s="8" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="M182" s="8" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="183" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -13035,10 +13131,10 @@
         <v>1182</v>
       </c>
       <c r="L183" s="8" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="M183" s="8" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="184" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -13068,10 +13164,10 @@
         <v>1184</v>
       </c>
       <c r="L184" s="8" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="M184" s="8" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="185" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -13101,10 +13197,10 @@
         <v>1186</v>
       </c>
       <c r="L185" s="8" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="M185" s="8" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="186" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13126,7 +13222,7 @@
       </c>
       <c r="K186" s="19"/>
       <c r="L186" s="25" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="M186" s="19"/>
     </row>
@@ -13157,10 +13253,10 @@
         <v>1189</v>
       </c>
       <c r="L187" s="8" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="M187" s="8" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="188" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -13190,10 +13286,10 @@
         <v>971</v>
       </c>
       <c r="L188" s="8" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="M188" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="189" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13215,7 +13311,7 @@
       </c>
       <c r="K189" s="19"/>
       <c r="L189" s="25" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="M189" s="19"/>
     </row>
@@ -13246,10 +13342,10 @@
         <v>1193</v>
       </c>
       <c r="L190" s="8" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="M190" s="8" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="191" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -13279,10 +13375,10 @@
         <v>1195</v>
       </c>
       <c r="L191" s="8" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="M191" s="8" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="192" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -13304,7 +13400,7 @@
       </c>
       <c r="K192" s="19"/>
       <c r="L192" s="25" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="M192" s="19"/>
     </row>
@@ -13335,10 +13431,10 @@
         <v>971</v>
       </c>
       <c r="L193" s="8" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="M193" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="194" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -13368,10 +13464,10 @@
         <v>1199</v>
       </c>
       <c r="L194" s="8" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
       <c r="M194" s="8" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="195" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -13401,10 +13497,10 @@
         <v>971</v>
       </c>
       <c r="L195" s="8" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="M195" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="196" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13426,7 +13522,7 @@
       </c>
       <c r="K196" s="19"/>
       <c r="L196" s="25" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
       <c r="M196" s="19"/>
     </row>
@@ -13457,10 +13553,10 @@
         <v>971</v>
       </c>
       <c r="L197" s="8" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
       <c r="M197" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="198" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -13490,10 +13586,10 @@
         <v>971</v>
       </c>
       <c r="L198" s="8" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
       <c r="M198" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="199" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -13523,10 +13619,10 @@
         <v>971</v>
       </c>
       <c r="L199" s="8" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="M199" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="200" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -13548,7 +13644,7 @@
       </c>
       <c r="K200" s="19"/>
       <c r="L200" s="25" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
       <c r="M200" s="19"/>
     </row>
@@ -13579,10 +13675,10 @@
         <v>1403</v>
       </c>
       <c r="L201" s="8" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
       <c r="M201" s="8" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="202" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -13612,10 +13708,10 @@
         <v>1208</v>
       </c>
       <c r="L202" s="8" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="M202" s="8" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="203" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -13637,7 +13733,7 @@
       </c>
       <c r="K203" s="19"/>
       <c r="L203" s="25" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="M203" s="19"/>
     </row>
@@ -13668,10 +13764,10 @@
         <v>1211</v>
       </c>
       <c r="L204" s="8" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="M204" s="8" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="205" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -13701,10 +13797,10 @@
         <v>1213</v>
       </c>
       <c r="L205" s="8" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="M205" s="8" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="206" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13726,7 +13822,7 @@
       </c>
       <c r="K206" s="19"/>
       <c r="L206" s="25" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="M206" s="19"/>
     </row>
@@ -13756,10 +13852,10 @@
         <v>1216</v>
       </c>
       <c r="L207" s="8" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
       <c r="M207" s="8" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="208" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -13786,10 +13882,10 @@
         <v>927</v>
       </c>
       <c r="K208" s="16" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
       <c r="L208" s="24" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="M208" s="16"/>
     </row>
@@ -13812,7 +13908,7 @@
       </c>
       <c r="K209" s="19"/>
       <c r="L209" s="25" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="M209" s="19"/>
     </row>
@@ -13843,10 +13939,10 @@
         <v>1404</v>
       </c>
       <c r="L210" s="8" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
       <c r="M210" s="8" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="129.6" x14ac:dyDescent="0.3">
@@ -13876,10 +13972,10 @@
         <v>1405</v>
       </c>
       <c r="L211" s="8" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
       <c r="M211" s="8" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="212" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -13909,10 +14005,10 @@
         <v>1222</v>
       </c>
       <c r="L212" s="8" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="M212" s="8" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="213" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -13969,10 +14065,10 @@
         <v>1224</v>
       </c>
       <c r="L214" s="8" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="M214" s="8" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="215" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -14002,10 +14098,10 @@
         <v>971</v>
       </c>
       <c r="L215" s="8" t="s">
-        <v>1824</v>
+        <v>1822</v>
       </c>
       <c r="M215" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="216" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -14035,10 +14131,10 @@
         <v>971</v>
       </c>
       <c r="L216" s="8" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="M216" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="217" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14060,7 +14156,7 @@
       </c>
       <c r="K217" s="19"/>
       <c r="L217" s="25" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="M217" s="19"/>
     </row>
@@ -14091,10 +14187,10 @@
         <v>971</v>
       </c>
       <c r="L218" s="8" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="M218" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="219" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -14124,10 +14220,10 @@
         <v>971</v>
       </c>
       <c r="L219" s="8" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="M219" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -14156,10 +14252,10 @@
         <v>971</v>
       </c>
       <c r="L220" s="8" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="M220" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="221" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -14186,10 +14282,10 @@
         <v>927</v>
       </c>
       <c r="K221" s="16" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="L221" s="24" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
       <c r="M221" s="16"/>
     </row>
@@ -14212,7 +14308,7 @@
       </c>
       <c r="K222" s="19"/>
       <c r="L222" s="25" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="M222" s="19"/>
     </row>
@@ -14243,10 +14339,10 @@
         <v>1232</v>
       </c>
       <c r="L223" s="8" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="M223" s="8" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="224" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -14276,10 +14372,10 @@
         <v>1234</v>
       </c>
       <c r="L224" s="8" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="M224" s="8" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="225" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -14309,10 +14405,10 @@
         <v>1236</v>
       </c>
       <c r="L225" s="8" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="M225" s="8" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="226" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -14342,10 +14438,10 @@
         <v>971</v>
       </c>
       <c r="L226" s="8" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="M226" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="227" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14367,7 +14463,7 @@
       </c>
       <c r="K227" s="19"/>
       <c r="L227" s="25" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="M227" s="19"/>
     </row>
@@ -14398,10 +14494,10 @@
         <v>971</v>
       </c>
       <c r="L228" s="8" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="M228" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="229" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -14431,10 +14527,10 @@
         <v>971</v>
       </c>
       <c r="L229" s="8" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="M229" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="230" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -14464,10 +14560,10 @@
         <v>1241</v>
       </c>
       <c r="L230" s="8" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="M230" s="8" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="231" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -14489,7 +14585,7 @@
       </c>
       <c r="K231" s="19"/>
       <c r="L231" s="25" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="M231" s="19"/>
     </row>
@@ -14520,10 +14616,10 @@
         <v>1244</v>
       </c>
       <c r="L232" s="8" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
       <c r="M232" s="8" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="233" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -14553,10 +14649,10 @@
         <v>971</v>
       </c>
       <c r="L233" s="8" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="M233" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="234" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -14586,10 +14682,10 @@
         <v>971</v>
       </c>
       <c r="L234" s="8" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="M234" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="235" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14611,7 +14707,7 @@
       </c>
       <c r="K235" s="19"/>
       <c r="L235" s="25" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="M235" s="19"/>
     </row>
@@ -14642,10 +14738,10 @@
         <v>1249</v>
       </c>
       <c r="L236" s="8" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="M236" s="8" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="237" spans="1:13" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -14675,10 +14771,10 @@
         <v>1251</v>
       </c>
       <c r="L237" s="8" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
       <c r="M237" s="8" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="238" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -14707,10 +14803,10 @@
         <v>971</v>
       </c>
       <c r="L238" s="8" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
       <c r="M238" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="239" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -14733,7 +14829,7 @@
         <v>927</v>
       </c>
       <c r="K239" s="12" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
       <c r="L239" s="23"/>
       <c r="M239" s="12"/>
@@ -14762,10 +14858,10 @@
         <v>927</v>
       </c>
       <c r="K240" s="16" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="L240" s="24" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="M240" s="16"/>
     </row>
@@ -14788,7 +14884,7 @@
       </c>
       <c r="K241" s="19"/>
       <c r="L241" s="25" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="M241" s="19"/>
     </row>
@@ -14819,10 +14915,10 @@
         <v>1256</v>
       </c>
       <c r="L242" s="8" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="M242" s="8" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="243" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14844,7 +14940,7 @@
       </c>
       <c r="K243" s="19"/>
       <c r="L243" s="25" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="M243" s="19"/>
     </row>
@@ -14875,10 +14971,10 @@
         <v>971</v>
       </c>
       <c r="L244" s="8" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="M244" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="245" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -14908,10 +15004,10 @@
         <v>1260</v>
       </c>
       <c r="L245" s="8" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="M245" s="8" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="246" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -14933,7 +15029,7 @@
       </c>
       <c r="K246" s="19"/>
       <c r="L246" s="25" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="M246" s="19"/>
     </row>
@@ -14964,10 +15060,10 @@
         <v>1262</v>
       </c>
       <c r="L247" s="8" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
       <c r="M247" s="8" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="248" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -14997,10 +15093,10 @@
         <v>971</v>
       </c>
       <c r="L248" s="8" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="M248" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="249" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -15030,10 +15126,10 @@
         <v>971</v>
       </c>
       <c r="L249" s="8" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="M249" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="250" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -15055,7 +15151,7 @@
       </c>
       <c r="K250" s="19"/>
       <c r="L250" s="25" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="M250" s="19"/>
     </row>
@@ -15086,10 +15182,10 @@
         <v>971</v>
       </c>
       <c r="L251" s="8" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="M251" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="252" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -15111,7 +15207,7 @@
       </c>
       <c r="K252" s="19"/>
       <c r="L252" s="25" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="M252" s="19"/>
     </row>
@@ -15142,10 +15238,10 @@
         <v>971</v>
       </c>
       <c r="L253" s="8" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="M253" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="254" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -15175,10 +15271,10 @@
         <v>971</v>
       </c>
       <c r="L254" s="8" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="M254" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="255" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -15205,10 +15301,10 @@
         <v>927</v>
       </c>
       <c r="K255" s="16" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="L255" s="24" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="M255" s="16"/>
     </row>
@@ -15231,7 +15327,7 @@
       </c>
       <c r="K256" s="19"/>
       <c r="L256" s="25" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="M256" s="19"/>
     </row>
@@ -15262,10 +15358,10 @@
         <v>1274</v>
       </c>
       <c r="L257" s="8" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="M257" s="8" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="258" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
@@ -15295,10 +15391,10 @@
         <v>1275</v>
       </c>
       <c r="L258" s="8" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="M258" s="8" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="259" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
@@ -15328,10 +15424,10 @@
         <v>1277</v>
       </c>
       <c r="L259" s="8" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
       <c r="M259" s="8" t="s">
-        <v>1884</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="260" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15353,41 +15449,41 @@
       </c>
       <c r="K260" s="19"/>
       <c r="L260" s="25" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="M260" s="19"/>
     </row>
-    <row r="261" spans="1:13" s="33" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A261" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="B261" s="33">
-        <v>4</v>
-      </c>
-      <c r="C261" s="33" t="s">
+    <row r="261" spans="1:13" s="31" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A261" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B261" s="31">
+        <v>4</v>
+      </c>
+      <c r="C261" s="31" t="s">
         <v>882</v>
       </c>
-      <c r="D261" s="33" t="s">
+      <c r="D261" s="31" t="s">
         <v>627</v>
       </c>
-      <c r="F261" s="34" t="s">
+      <c r="F261" s="32" t="s">
         <v>628</v>
       </c>
-      <c r="G261" s="34" t="s">
+      <c r="G261" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="I261" s="35" t="s">
+      <c r="I261" s="33" t="s">
         <v>1279</v>
       </c>
-      <c r="J261" s="35" t="s">
+      <c r="J261" s="33" t="s">
         <v>971</v>
       </c>
-      <c r="K261" s="35"/>
-      <c r="L261" s="36" t="s">
-        <v>1885</v>
-      </c>
-      <c r="M261" s="35" t="s">
-        <v>1510</v>
+      <c r="K261" s="33"/>
+      <c r="L261" s="34" t="s">
+        <v>1883</v>
+      </c>
+      <c r="M261" s="33" t="s">
+        <v>1508</v>
       </c>
     </row>
     <row r="262" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -15417,10 +15513,10 @@
         <v>1281</v>
       </c>
       <c r="L262" s="8" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="M262" s="8" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="263" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15442,7 +15538,7 @@
       </c>
       <c r="K263" s="19"/>
       <c r="L263" s="25" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="M263" s="19"/>
     </row>
@@ -15473,10 +15569,10 @@
         <v>1284</v>
       </c>
       <c r="L264" s="8" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
       <c r="M264" s="8" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="265" spans="1:13" ht="115.2" x14ac:dyDescent="0.3">
@@ -15506,10 +15602,10 @@
         <v>1286</v>
       </c>
       <c r="L265" s="8" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="M265" s="8" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="266" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -15539,10 +15635,10 @@
         <v>1288</v>
       </c>
       <c r="L266" s="8" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="M266" s="8" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="267" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -15564,7 +15660,7 @@
       </c>
       <c r="K267" s="19"/>
       <c r="L267" s="25" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="M267" s="19"/>
     </row>
@@ -15595,10 +15691,10 @@
         <v>1290</v>
       </c>
       <c r="L268" s="8" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="M268" s="8" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="269" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -15628,10 +15724,10 @@
         <v>971</v>
       </c>
       <c r="L269" s="8" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="M269" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="270" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -15653,7 +15749,7 @@
       </c>
       <c r="K270" s="19"/>
       <c r="L270" s="25" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="M270" s="19"/>
     </row>
@@ -15684,10 +15780,10 @@
         <v>1294</v>
       </c>
       <c r="L271" s="8" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="M271" s="8" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="272" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15709,7 +15805,7 @@
       </c>
       <c r="K272" s="19"/>
       <c r="L272" s="25" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="M272" s="19"/>
     </row>
@@ -15740,10 +15836,10 @@
         <v>1297</v>
       </c>
       <c r="L273" s="8" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
       <c r="M273" s="8" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="274" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -15773,10 +15869,10 @@
         <v>971</v>
       </c>
       <c r="L274" s="8" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="M274" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="275" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -15798,7 +15894,7 @@
       </c>
       <c r="K275" s="19"/>
       <c r="L275" s="25" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="M275" s="19"/>
     </row>
@@ -15829,10 +15925,10 @@
         <v>1301</v>
       </c>
       <c r="L276" s="8" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="M276" s="8" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="277" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -15862,10 +15958,10 @@
         <v>971</v>
       </c>
       <c r="L277" s="8" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="M277" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="278" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -15887,7 +15983,7 @@
       </c>
       <c r="K278" s="19"/>
       <c r="L278" s="25" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="M278" s="19"/>
     </row>
@@ -15918,10 +16014,10 @@
         <v>1305</v>
       </c>
       <c r="L279" s="8" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="M279" s="8" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="280" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -15951,10 +16047,10 @@
         <v>971</v>
       </c>
       <c r="L280" s="8" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="M280" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="281" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -15981,10 +16077,10 @@
         <v>927</v>
       </c>
       <c r="K281" s="16" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="L281" s="24" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="M281" s="16"/>
     </row>
@@ -16007,7 +16103,7 @@
       </c>
       <c r="K282" s="19"/>
       <c r="L282" s="25" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="M282" s="19"/>
     </row>
@@ -16038,10 +16134,10 @@
         <v>971</v>
       </c>
       <c r="L283" s="8" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="M283" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="284" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -16063,7 +16159,7 @@
       </c>
       <c r="K284" s="19"/>
       <c r="L284" s="25" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="M284" s="19"/>
     </row>
@@ -16094,10 +16190,10 @@
         <v>1313</v>
       </c>
       <c r="L285" s="8" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="M285" s="8" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="286" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16119,7 +16215,7 @@
       </c>
       <c r="K286" s="19"/>
       <c r="L286" s="25" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="M286" s="19"/>
     </row>
@@ -16150,10 +16246,10 @@
         <v>1316</v>
       </c>
       <c r="L287" s="8" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="M287" s="8" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="288" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16175,7 +16271,7 @@
       </c>
       <c r="K288" s="19"/>
       <c r="L288" s="25" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="M288" s="19"/>
     </row>
@@ -16206,10 +16302,10 @@
         <v>1319</v>
       </c>
       <c r="L289" s="8" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="M289" s="8" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="290" spans="1:13" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -16239,10 +16335,10 @@
         <v>1321</v>
       </c>
       <c r="L290" s="8" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="M290" s="8" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="291" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -16267,7 +16363,7 @@
         <v>927</v>
       </c>
       <c r="K291" s="12" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="L291" s="23"/>
       <c r="M291" s="12"/>
@@ -16296,10 +16392,10 @@
         <v>927</v>
       </c>
       <c r="K292" s="16" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="L292" s="24" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="M292" s="16"/>
     </row>
@@ -16322,7 +16418,7 @@
       </c>
       <c r="K293" s="19"/>
       <c r="L293" s="25" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="M293" s="19"/>
     </row>
@@ -16353,10 +16449,10 @@
         <v>1327</v>
       </c>
       <c r="L294" s="8" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
       <c r="M294" s="8" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="295" spans="1:13" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -16383,10 +16479,10 @@
         <v>927</v>
       </c>
       <c r="K295" s="16" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="L295" s="24" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="M295" s="16"/>
     </row>
@@ -16409,7 +16505,7 @@
       </c>
       <c r="K296" s="19"/>
       <c r="L296" s="25" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="M296" s="19"/>
     </row>
@@ -16440,10 +16536,10 @@
         <v>1331</v>
       </c>
       <c r="L297" s="8" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="M297" s="8" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="298" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16465,7 +16561,7 @@
       </c>
       <c r="K298" s="19"/>
       <c r="L298" s="25" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="M298" s="19"/>
     </row>
@@ -16496,10 +16592,10 @@
         <v>1334</v>
       </c>
       <c r="L299" s="8" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="M299" s="8" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="300" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -16529,10 +16625,10 @@
         <v>1336</v>
       </c>
       <c r="L300" s="8" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="M300" s="8" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="301" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16554,7 +16650,7 @@
       </c>
       <c r="K301" s="19"/>
       <c r="L301" s="25" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="M301" s="19"/>
     </row>
@@ -16585,10 +16681,10 @@
         <v>971</v>
       </c>
       <c r="L302" s="8" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="M302" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="303" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -16618,10 +16714,10 @@
         <v>971</v>
       </c>
       <c r="L303" s="8" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="M303" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="304" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16643,7 +16739,7 @@
       </c>
       <c r="K304" s="19"/>
       <c r="L304" s="25" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="M304" s="19"/>
     </row>
@@ -16674,10 +16770,10 @@
         <v>1342</v>
       </c>
       <c r="L305" s="8" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="M305" s="8" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="306" spans="1:13" s="17" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -16699,7 +16795,7 @@
       </c>
       <c r="K306" s="19"/>
       <c r="L306" s="25" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="M306" s="19"/>
     </row>
@@ -16730,10 +16826,10 @@
         <v>971</v>
       </c>
       <c r="L307" s="8" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="M307" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="308" spans="1:13" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -16763,7 +16859,7 @@
         <v>1345</v>
       </c>
       <c r="L308" s="24" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="M308" s="16"/>
     </row>
@@ -16786,7 +16882,7 @@
       </c>
       <c r="K309" s="19"/>
       <c r="L309" s="25" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="M309" s="19"/>
     </row>
@@ -16817,10 +16913,10 @@
         <v>971</v>
       </c>
       <c r="L310" s="8" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="M310" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="311" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -16850,10 +16946,10 @@
         <v>971</v>
       </c>
       <c r="L311" s="8" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="M311" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="312" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -16875,7 +16971,7 @@
       </c>
       <c r="K312" s="19"/>
       <c r="L312" s="25" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="M312" s="19"/>
     </row>
@@ -16906,10 +17002,10 @@
         <v>1352</v>
       </c>
       <c r="L313" s="8" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="M313" s="8" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="314" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -16939,10 +17035,10 @@
         <v>1354</v>
       </c>
       <c r="L314" s="8" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="M314" s="8" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="315" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -16964,7 +17060,7 @@
       </c>
       <c r="K315" s="19"/>
       <c r="L315" s="25" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="M315" s="19"/>
     </row>
@@ -16995,10 +17091,10 @@
         <v>971</v>
       </c>
       <c r="L316" s="8" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="M316" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="317" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -17028,10 +17124,10 @@
         <v>1358</v>
       </c>
       <c r="L317" s="8" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="M317" s="8" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="318" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -17053,7 +17149,7 @@
       </c>
       <c r="K318" s="19"/>
       <c r="L318" s="25" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="M318" s="19"/>
     </row>
@@ -17084,10 +17180,10 @@
         <v>1361</v>
       </c>
       <c r="L319" s="8" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="M319" s="8" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="320" spans="1:13" s="17" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -17109,7 +17205,7 @@
       </c>
       <c r="K320" s="19"/>
       <c r="L320" s="25" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="M320" s="19"/>
     </row>
@@ -17140,10 +17236,10 @@
         <v>971</v>
       </c>
       <c r="L321" s="8" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="M321" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="322" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -17173,10 +17269,10 @@
         <v>971</v>
       </c>
       <c r="L322" s="8" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="M322" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="323" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -17203,10 +17299,10 @@
         <v>927</v>
       </c>
       <c r="K323" s="16" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="L323" s="24" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="M323" s="16"/>
     </row>
@@ -17229,7 +17325,7 @@
       </c>
       <c r="K324" s="19"/>
       <c r="L324" s="25" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="M324" s="19"/>
     </row>
@@ -17253,19 +17349,19 @@
         <v>3</v>
       </c>
       <c r="D326" s="17" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="F326" s="18" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="G326" s="18"/>
       <c r="I326" s="19" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="J326" s="19"/>
       <c r="K326" s="19"/>
       <c r="L326" s="25" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="M326" s="19"/>
     </row>
@@ -17280,7 +17376,7 @@
         <v>882</v>
       </c>
       <c r="D327" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="H327"/>
     </row>
@@ -17289,19 +17385,19 @@
         <v>3</v>
       </c>
       <c r="D328" s="17" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="F328" s="18" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="G328" s="18"/>
       <c r="I328" s="19" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="J328" s="19"/>
       <c r="K328" s="19"/>
       <c r="L328" s="25" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="M328" s="19"/>
     </row>
@@ -17316,7 +17412,7 @@
         <v>882</v>
       </c>
       <c r="D329" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="F329" s="3" t="s">
         <v>782</v>
@@ -17332,10 +17428,10 @@
         <v>1368</v>
       </c>
       <c r="L329" s="8" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="M329" s="8" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="330" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -17362,10 +17458,10 @@
         <v>927</v>
       </c>
       <c r="K330" s="16" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="L330" s="24" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="M330" s="16"/>
     </row>
@@ -17388,7 +17484,7 @@
       </c>
       <c r="K331" s="19"/>
       <c r="L331" s="25" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="M331" s="19"/>
     </row>
@@ -17419,10 +17515,10 @@
         <v>1372</v>
       </c>
       <c r="L332" s="8" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="M332" s="8" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="333" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -17452,10 +17548,10 @@
         <v>971</v>
       </c>
       <c r="L333" s="8" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="M333" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="334" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -17477,7 +17573,7 @@
       </c>
       <c r="K334" s="19"/>
       <c r="L334" s="25" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="M334" s="19"/>
     </row>
@@ -17508,10 +17604,10 @@
         <v>1375</v>
       </c>
       <c r="L335" s="8" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="M335" s="8" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="336" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -17536,7 +17632,7 @@
         <v>927</v>
       </c>
       <c r="K336" s="12" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="L336" s="23"/>
       <c r="M336" s="12"/>
@@ -17565,10 +17661,10 @@
         <v>927</v>
       </c>
       <c r="K337" s="16" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="L337" s="24" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="M337" s="16"/>
     </row>
@@ -17591,7 +17687,7 @@
       </c>
       <c r="K338" s="19"/>
       <c r="L338" s="25" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="M338" s="19"/>
     </row>
@@ -17619,13 +17715,13 @@
         <v>1380</v>
       </c>
       <c r="J339" s="8" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="L339" s="8" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="M339" s="8" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="340" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -17655,10 +17751,10 @@
         <v>971</v>
       </c>
       <c r="L340" s="8" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="M340" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="341" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -17685,10 +17781,10 @@
         <v>927</v>
       </c>
       <c r="K341" s="16" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="L341" s="24" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="M341" s="16"/>
     </row>
@@ -17711,7 +17807,7 @@
       </c>
       <c r="K342" s="19"/>
       <c r="L342" s="25" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="M342" s="19"/>
     </row>
@@ -17742,10 +17838,10 @@
         <v>971</v>
       </c>
       <c r="L343" s="8" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="M343" s="8" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="344" spans="1:13" s="13" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -17772,10 +17868,10 @@
         <v>927</v>
       </c>
       <c r="K344" s="16" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="L344" s="24" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="M344" s="16"/>
     </row>
@@ -17798,7 +17894,7 @@
       </c>
       <c r="K345" s="19"/>
       <c r="L345" s="25" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="M345" s="19"/>
     </row>
@@ -17829,10 +17925,10 @@
         <v>1387</v>
       </c>
       <c r="L346" s="8" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="M346" s="8" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="347" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -17862,10 +17958,10 @@
         <v>1389</v>
       </c>
       <c r="L347" s="8" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="M347" s="8" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="348" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -17887,7 +17983,7 @@
       </c>
       <c r="K348" s="19"/>
       <c r="L348" s="25" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="M348" s="19"/>
     </row>
@@ -17918,10 +18014,10 @@
         <v>1392</v>
       </c>
       <c r="L349" s="8" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="M349" s="8" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="350" spans="1:13" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -17943,7 +18039,7 @@
       </c>
       <c r="K350" s="19"/>
       <c r="L350" s="25" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="M350" s="19"/>
     </row>
@@ -17974,10 +18070,10 @@
         <v>1395</v>
       </c>
       <c r="L351" s="8" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="M351" s="8" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
     </row>
   </sheetData>
@@ -17992,10 +18088,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8EE66F-5BF1-6F47-9F88-8D8C53839AC6}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18006,10 +18102,13 @@
     <col min="5" max="5" width="10.77734375" style="3"/>
     <col min="6" max="6" width="46.109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="50.33203125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="10.77734375" style="3"/>
+    <col min="8" max="8" width="17.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="46.109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="50.33203125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="10.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>867</v>
       </c>
@@ -18031,8 +18130,17 @@
       <c r="G1" s="21" t="s">
         <v>1467</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H1" s="21" t="s">
+        <v>1487</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>1488</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -18054,8 +18162,17 @@
       <c r="G2" s="3" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H2" s="3" t="s">
+        <v>2024</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>2029</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -18077,8 +18194,17 @@
       <c r="G3" s="3" t="s">
         <v>1455</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="H3" s="3" t="s">
+        <v>2025</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2030</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -18086,7 +18212,7 @@
         <v>870</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1445</v>
@@ -18095,13 +18221,22 @@
         <v>1449</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>1456</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="H4" s="3" t="s">
+        <v>2026</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2031</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -18109,7 +18244,7 @@
         <v>871</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1446</v>
@@ -18118,13 +18253,22 @@
         <v>1450</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>1457</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="H5" s="3" t="s">
+        <v>2027</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>2032</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -18132,7 +18276,7 @@
         <v>872</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1447</v>
@@ -18141,23 +18285,33 @@
         <v>1451</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>1458</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>2028</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>2033</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>2038</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793A9884-A8FA-0245-8718-D92EEEA60D41}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18167,7 +18321,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>837</v>
       </c>
@@ -18183,8 +18337,14 @@
       <c r="E1" s="20" t="s">
         <v>1397</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="20" t="s">
+        <v>1487</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>875</v>
       </c>
@@ -18194,8 +18354,11 @@
       <c r="D2" t="s">
         <v>1459</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>876</v>
       </c>
@@ -18205,8 +18368,11 @@
       <c r="D3" t="s">
         <v>879</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>877</v>
       </c>
@@ -18216,8 +18382,11 @@
       <c r="D4" t="s">
         <v>1460</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>886</v>
       </c>
@@ -18227,8 +18396,11 @@
       <c r="D5" t="s">
         <v>1461</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>887</v>
       </c>
@@ -18238,8 +18410,11 @@
       <c r="D6" t="s">
         <v>1462</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>888</v>
       </c>
@@ -18248,6 +18423,9 @@
       </c>
       <c r="D7" t="s">
         <v>1463</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>